<commit_message>
Addition of Part 2 of the Project
- Added more charts to the Excel Sheet
- Added Part 2
- Added the Possible Extra Credit Sheet
</commit_message>
<xml_diff>
--- a/Project2/Part_2/Rainbow Six Siege Stats.xlsx
+++ b/Project2/Part_2/Rainbow Six Siege Stats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Add Thunderbird, Osa, Thorn, Az" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Operator</t>
   </si>
@@ -46,7 +46,13 @@
     <t>Ash</t>
   </si>
   <si>
+    <t>Median of Kills:</t>
+  </si>
+  <si>
     <t>Jäger</t>
+  </si>
+  <si>
+    <t>Average Deaths:</t>
   </si>
   <si>
     <t>Bandit</t>
@@ -233,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -243,6 +249,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -251,8 +258,906 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Deaths</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet 1'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet 1'!$E$2:$E$58</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="36139174"/>
+        <c:axId val="404247513"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="36139174"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404247513"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="404247513"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Deaths</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="36139174"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Kills</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet 1'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F9CB9C"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet 1'!$A$3:$A$58</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet 1'!$D$2:$D$58</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="1537538424"/>
+        <c:axId val="1426603818"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1537538424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1426603818"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1426603818"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Kills</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1537538424"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet 1'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet 1'!$A$2:$A$58</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet 1'!$B$2:$B$58</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet 1'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet 1'!$A$2:$A$58</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet 1'!$C$2:$C$58</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet 1'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet 1'!$A$2:$A$58</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet 1'!$D$2:$D$58</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet 1'!$E$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet 1'!$A$2:$A$58</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet 1'!$E$2:$E$58</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet 1'!$F$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet 1'!$A$2:$A$58</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet 1'!$F$2:$F$58</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="100"/>
+        <c:axId val="1746559403"/>
+        <c:axId val="804861380"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1746559403"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="804861380"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="804861380"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1746559403"/>
+        <c:crosses val="max"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9210675" cy="5695950"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6924675" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,6 +1363,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="9" max="9" width="14.5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -578,10 +1486,17 @@
       <c r="F6" s="2">
         <v>0.5797</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="3">
+        <f>MEDIAN(D2:D58)</f>
+        <v>277</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>312.0</v>
@@ -598,10 +1513,17 @@
       <c r="F7" s="2">
         <v>0.5769</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="3">
+        <f>AVERAGE(E2:E58)</f>
+        <v>203.2982456</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1">
         <v>215.0</v>
@@ -621,7 +1543,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>295.0</v>
@@ -641,7 +1563,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>11.0</v>
@@ -661,7 +1583,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>23.0</v>
@@ -681,7 +1603,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
         <v>258.0</v>
@@ -701,7 +1623,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1">
         <v>207.0</v>
@@ -721,7 +1643,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>189.0</v>
@@ -741,7 +1663,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>231.0</v>
@@ -761,7 +1683,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>263.0</v>
@@ -781,7 +1703,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1">
         <v>291.0</v>
@@ -801,7 +1723,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1">
         <v>302.0</v>
@@ -821,7 +1743,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1">
         <v>255.0</v>
@@ -841,7 +1763,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1">
         <v>229.0</v>
@@ -861,7 +1783,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1">
         <v>288.0</v>
@@ -881,7 +1803,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1">
         <v>322.0</v>
@@ -901,7 +1823,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1">
         <v>243.0</v>
@@ -921,7 +1843,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1">
         <v>271.0</v>
@@ -941,7 +1863,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>239.0</v>
@@ -961,7 +1883,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1">
         <v>267.0</v>
@@ -981,7 +1903,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1">
         <v>219.0</v>
@@ -1001,7 +1923,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1">
         <v>252.0</v>
@@ -1021,7 +1943,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1">
         <v>297.0</v>
@@ -1041,7 +1963,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1">
         <v>204.0</v>
@@ -1061,7 +1983,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1">
         <v>317.0</v>
@@ -1081,7 +2003,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1">
         <v>345.0</v>
@@ -1101,7 +2023,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1">
         <v>285.0</v>
@@ -1121,7 +2043,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B34" s="1">
         <v>269.0</v>
@@ -1141,7 +2063,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1">
         <v>222.0</v>
@@ -1161,7 +2083,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1">
         <v>308.0</v>
@@ -1181,7 +2103,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1">
         <v>249.0</v>
@@ -1201,7 +2123,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1">
         <v>278.0</v>
@@ -1221,7 +2143,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1">
         <v>212.0</v>
@@ -1241,7 +2163,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1">
         <v>325.0</v>
@@ -1261,7 +2183,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B41" s="1">
         <v>257.0</v>
@@ -1281,7 +2203,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B42" s="1">
         <v>293.0</v>
@@ -1301,7 +2223,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B43" s="1">
         <v>47.0</v>
@@ -1321,7 +2243,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1">
         <v>280.0</v>
@@ -1341,7 +2263,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B45" s="1">
         <v>245.0</v>
@@ -1361,7 +2283,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B46" s="1">
         <v>262.0</v>
@@ -1381,7 +2303,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B47" s="1">
         <v>298.0</v>
@@ -1401,7 +2323,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B48" s="1">
         <v>210.0</v>
@@ -1421,7 +2343,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1">
         <v>275.0</v>
@@ -1441,7 +2363,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B50" s="1">
         <v>250.0</v>
@@ -1461,7 +2383,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B51" s="1">
         <v>220.0</v>
@@ -1481,7 +2403,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B52" s="1">
         <v>285.0</v>
@@ -1501,7 +2423,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B53" s="1">
         <v>240.0</v>
@@ -1521,7 +2443,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B54" s="1">
         <v>265.0</v>
@@ -1541,7 +2463,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1">
         <v>215.0</v>
@@ -1561,7 +2483,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B56" s="1">
         <v>290.0</v>
@@ -1581,7 +2503,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B57" s="1">
         <v>235.0</v>
@@ -1601,7 +2523,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B58" s="1">
         <v>275.0</v>

</xml_diff>